<commit_message>
some changes in task3
</commit_message>
<xml_diff>
--- a/dbms/Problems 2.xlsx
+++ b/dbms/Problems 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\engpract_sem3\Homework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\engpract_sem3\dbms\dbms\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -198,44 +198,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>37824</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>434340</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>54410</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1394460" y="9364704"/>
-          <a:ext cx="6355080" cy="3857066"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
       <xdr:colOff>281940</xdr:colOff>
       <xdr:row>126</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -254,7 +216,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -292,7 +254,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -330,7 +292,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -368,7 +330,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -406,7 +368,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -444,7 +406,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -482,7 +444,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -520,7 +482,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -558,7 +520,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -596,7 +558,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -605,6 +567,44 @@
         <a:xfrm>
           <a:off x="1699261" y="44028361"/>
           <a:ext cx="5280660" cy="1440180"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>93633</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>127449</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Рисунок 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1569720" y="9603393"/>
+          <a:ext cx="7970520" cy="3691416"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -915,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A227" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C249" sqref="C249"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R62" sqref="R62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>